<commit_message>
Create the intuitive APIs for operating Excel. Support XLS and XLSX.
</commit_message>
<xml_diff>
--- a/simoncat-framework-document-operator/src/test/resources/test.xlsx
+++ b/simoncat-framework-document-operator/src/test/resources/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>aa</t>
   </si>
@@ -33,6 +33,60 @@
   </si>
   <si>
     <t>2cc</t>
+  </si>
+  <si>
+    <t>aa_modified</t>
+  </si>
+  <si>
+    <t>bb_modified</t>
+  </si>
+  <si>
+    <t>cc_modified</t>
+  </si>
+  <si>
+    <t>2aa_modified</t>
+  </si>
+  <si>
+    <t>2bb_modified</t>
+  </si>
+  <si>
+    <t>2cc_modified</t>
+  </si>
+  <si>
+    <t>aa_modified_modified</t>
+  </si>
+  <si>
+    <t>bb_modified_modified</t>
+  </si>
+  <si>
+    <t>cc_modified_modified</t>
+  </si>
+  <si>
+    <t>2aa_modified_modified</t>
+  </si>
+  <si>
+    <t>2bb_modified_modified</t>
+  </si>
+  <si>
+    <t>2cc_modified_modified</t>
+  </si>
+  <si>
+    <t>aa_modified_modified_modified</t>
+  </si>
+  <si>
+    <t>bb_modified_modified_modified</t>
+  </si>
+  <si>
+    <t>cc_modified_modified_modified</t>
+  </si>
+  <si>
+    <t>2aa_modified_modified_modified</t>
+  </si>
+  <si>
+    <t>2bb_modified_modified_modified</t>
+  </si>
+  <si>
+    <t>2cc_modified_modified_modified</t>
   </si>
 </sst>
 </file>
@@ -47,6 +101,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -131,34 +186,34 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col min="1" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>